<commit_message>
Ajuste o main e limpe os arquivos desnecessários
</commit_message>
<xml_diff>
--- a/Web_scraping/planilha_carteira.xlsx
+++ b/Web_scraping/planilha_carteira.xlsx
@@ -152,6 +152,36 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>7</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1257300" cy="1257300"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -645,5 +675,6 @@
     <mergeCell ref="E1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>